<commit_message>
Added Unix Script for Plotting Graphs
Implemented Unix scripts to generate various graphs including price changes over date, hourly stock trends and average price by category over date on Shoppu. The scripts efficiently parse and manipulate data to create insightful visual representations. This commit contributes to the project's goal of data visualization using Unix tools.
</commit_message>
<xml_diff>
--- a/docs/Timeline.xlsx
+++ b/docs/Timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\OneDrive - University of Southampton\UOSM\Year 1\Y1 S2\DM\5. COURSEWORK\DM CW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/bwkt1n22_soton_ac_uk/Documents/Projects/Others/OnlinePromotionStoreTracker/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2AA2602-7EDD-4442-B05C-0B99599759F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{F2AA2602-7EDD-4442-B05C-0B99599759F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C17A9064-E344-44BC-8A5F-659F46819278}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C6B9A78B-DE74-4D61-B461-09B04DE39BBE}"/>
+    <workbookView minimized="1" xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{C6B9A78B-DE74-4D61-B461-09B04DE39BBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,48 +179,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,12 +538,12 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection sqref="A1:Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="11.5546875" customWidth="1"/>
     <col min="3" max="4" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="6.77734375" bestFit="1" customWidth="1"/>
@@ -551,344 +551,344 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="3" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <v>45411</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <v>45412</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>45413</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <v>45414</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="3">
         <v>45415</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
         <v>45416</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="3">
         <v>45417</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="4">
         <v>45418</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="4">
         <v>45419</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="4">
         <v>45420</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="4">
         <v>45421</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="4">
         <v>45422</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="4">
         <v>45423</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="4">
         <v>45424</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="4">
         <v>45425</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
     </row>
     <row r="4" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
     </row>
     <row r="6" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:17" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="12"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="12"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="12"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="12"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="10"/>
     </row>
     <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="13"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>